<commit_message>
updated write up with formatted images
</commit_message>
<xml_diff>
--- a/output2.xlsx
+++ b/output2.xlsx
@@ -467,10 +467,10 @@
         <v>0.6666666666666667</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.666666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -481,13 +481,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.814814814814815</v>
+        <v>0.5925925925925927</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5185185185185188</v>
+        <v>0.07407407407407407</v>
       </c>
       <c r="E3" t="n">
-        <v>4.666666666666666</v>
+        <v>2.333333333333333</v>
       </c>
     </row>
     <row r="4">
@@ -498,13 +498,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6739826245999087</v>
+        <v>0.577960676726109</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.3776863283036125</v>
+        <v>0.01463191586648377</v>
       </c>
       <c r="E4" t="n">
-        <v>5.703703703703704</v>
+        <v>2.407407407407407</v>
       </c>
     </row>
     <row r="5">
@@ -515,13 +515,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7588339655417659</v>
+        <v>0.5751417860607781</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2928349873617553</v>
+        <v>0.002818890665330817</v>
       </c>
       <c r="E5" t="n">
-        <v>4.948331047096479</v>
+        <v>2.422039323273891</v>
       </c>
     </row>
     <row r="6">
@@ -532,13 +532,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6847629206387347</v>
+        <v>0.5746013654567886</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.2187639424587241</v>
+        <v>0.0005404206039894737</v>
       </c>
       <c r="E6" t="n">
-        <v>5.534001021819989</v>
+        <v>2.424858213939221</v>
       </c>
     </row>
     <row r="7">
@@ -549,13 +549,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7346967326948947</v>
+        <v>0.5744978566511308</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1688301304025641</v>
+        <v>0.000103508805657778</v>
       </c>
       <c r="E7" t="n">
-        <v>5.096473136902541</v>
+        <v>2.425398634543211</v>
       </c>
     </row>
     <row r="8">
@@ -566,13 +566,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6933504176324891</v>
+        <v>0.5744780347887992</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1274838153401585</v>
+        <v>1.98218623316373e-05</v>
       </c>
       <c r="E8" t="n">
-        <v>5.43413339770767</v>
+        <v>2.425502143348869</v>
       </c>
     </row>
     <row r="9">
@@ -583,13 +583,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7228140698349831</v>
+        <v>0.5744742390472932</v>
       </c>
       <c r="D9" t="n">
-        <v>0.09802016313766451</v>
+        <v>3.795741506044375e-06</v>
       </c>
       <c r="E9" t="n">
-        <v>5.179165767027353</v>
+        <v>2.4255219652112</v>
       </c>
     </row>
     <row r="10">
@@ -600,13 +600,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.699197285487175</v>
+        <v>0.5744735121953888</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.07440337878985642</v>
+        <v>7.268519044350228e-07</v>
       </c>
       <c r="E10" t="n">
-        <v>5.375206093302682</v>
+        <v>2.425525760952706</v>
       </c>
     </row>
     <row r="11">
@@ -617,13 +617,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7165381656474888</v>
+        <v>0.5744733730096666</v>
       </c>
       <c r="D11" t="n">
-        <v>0.05706249862954255</v>
+        <v>1.391857221288983e-07</v>
       </c>
       <c r="E11" t="n">
-        <v>5.226399335722969</v>
+        <v>2.425526487804611</v>
       </c>
     </row>
     <row r="12">
@@ -634,13 +634,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7029090129490639</v>
+        <v>0.5744733463568362</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.04343334593111763</v>
+        <v>2.665283042205812e-08</v>
       </c>
       <c r="E12" t="n">
-        <v>5.340524332982055</v>
+        <v>2.425526626990333</v>
       </c>
     </row>
     <row r="13">
@@ -651,13 +651,13 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7130855763882363</v>
+        <v>0.574473341253056</v>
       </c>
       <c r="D13" t="n">
-        <v>0.03325678249194525</v>
+        <v>5.10378022748034e-09</v>
       </c>
       <c r="E13" t="n">
-        <v>5.253657641119819</v>
+        <v>2.425526653643163</v>
       </c>
     </row>
     <row r="14">
@@ -668,13 +668,13 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7051805990842074</v>
+        <v>0.5744733402757275</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.02535180518791625</v>
+        <v>9.773285601006379e-10</v>
       </c>
       <c r="E14" t="n">
-        <v>5.320171206103709</v>
+        <v>2.425526658746943</v>
       </c>
     </row>
     <row r="15">
@@ -685,13 +685,13 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7111397994743011</v>
+        <v>0.5744733400885778</v>
       </c>
       <c r="D15" t="n">
-        <v>0.01939260479782261</v>
+        <v>1.871497341559602e-10</v>
       </c>
       <c r="E15" t="n">
-        <v>5.269467595727876</v>
+        <v>2.425526659724272</v>
       </c>
     </row>
     <row r="16">
@@ -702,13 +702,13 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7065428484452317</v>
+        <v>0.5744733400527402</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.0147956537687533</v>
+        <v>3.583751095908795e-11</v>
       </c>
       <c r="E16" t="n">
-        <v>5.308252805323522</v>
+        <v>2.425526659911422</v>
       </c>
     </row>
     <row r="17">
@@ -719,13 +719,13 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7100274362313599</v>
+        <v>0.5744733400458777</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01131106598262517</v>
+        <v>6.862564873281314e-12</v>
       </c>
       <c r="E17" t="n">
-        <v>5.278661497786016</v>
+        <v>2.425526659947259</v>
       </c>
     </row>
     <row r="18">
@@ -736,13 +736,13 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7073503805044642</v>
+        <v>0.5744733400445635</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.008634010255729473</v>
+        <v>1.31412018801181e-12</v>
       </c>
       <c r="E18" t="n">
-        <v>5.301283629751266</v>
+        <v>2.425526659954122</v>
       </c>
     </row>
     <row r="19">
@@ -753,13 +753,13 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>0.7093861373176874</v>
+        <v>0.5744733400443118</v>
       </c>
       <c r="D19" t="n">
-        <v>0.006598253442506244</v>
+        <v>2.516423378757115e-13</v>
       </c>
       <c r="E19" t="n">
-        <v>5.284015609239807</v>
+        <v>2.425526659955436</v>
       </c>
     </row>
     <row r="20">
@@ -770,13 +770,13 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7078259008101465</v>
+        <v>0.5744733400442636</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.005038016934965365</v>
+        <v>4.818727144533974e-14</v>
       </c>
       <c r="E20" t="n">
-        <v>5.29721211612482</v>
+        <v>2.425526659955688</v>
       </c>
     </row>
     <row r="21">
@@ -787,13 +787,13 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0.7090145804352427</v>
+        <v>0.5744733400442544</v>
       </c>
       <c r="D21" t="n">
-        <v>0.003849337309869154</v>
+        <v>9.227434258274629e-15</v>
       </c>
       <c r="E21" t="n">
-        <v>5.287136082254889</v>
+        <v>2.425526659955736</v>
       </c>
     </row>
     <row r="22">
@@ -804,13 +804,13 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7081048350093392</v>
+        <v>0.5744733400442527</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.00293959188396562</v>
+        <v>1.766971659463268e-15</v>
       </c>
       <c r="E22" t="n">
-        <v>5.294834756874628</v>
+        <v>2.425526659955745</v>
       </c>
     </row>
     <row r="23">
@@ -821,13 +821,13 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0.7087986814180026</v>
+        <v>0.5744733400442523</v>
       </c>
       <c r="D23" t="n">
-        <v>0.002245745475302197</v>
+        <v>3.383593703251331e-16</v>
       </c>
       <c r="E23" t="n">
-        <v>5.288955573106697</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="24">
@@ -838,13 +838,13 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7082680876074378</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.001715151664737316</v>
+        <v>6.479281253531642e-17</v>
       </c>
       <c r="E24" t="n">
-        <v>5.293447064057301</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="25">
@@ -855,13 +855,13 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0.7086730166706179</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D25" t="n">
-        <v>0.001310222601557246</v>
+        <v>1.240724780934144e-17</v>
       </c>
       <c r="E25" t="n">
-        <v>5.290016760727827</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="26">
@@ -872,13 +872,13 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.708363510202766</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.00100071613370538</v>
+        <v>2.375877696596369e-18</v>
       </c>
       <c r="E26" t="n">
-        <v>5.292637205930942</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="27">
@@ -889,13 +889,13 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>0.708599800467162</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0007644258693093519</v>
+        <v>4.5495946530012e-19</v>
       </c>
       <c r="E27" t="n">
-        <v>5.290635773663531</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="28">
@@ -906,13 +906,13 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>0.7084192431276738</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.0005838685298211709</v>
+        <v>8.712069453856902e-20</v>
       </c>
       <c r="E28" t="n">
-        <v>5.292164625402149</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="29">
@@ -923,13 +923,13 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>0.7085571176950011</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0004459939624938437</v>
+        <v>1.668283879284893e-20</v>
       </c>
       <c r="E29" t="n">
-        <v>5.290996888342507</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="30">
@@ -940,13 +940,13 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>0.7084517802961431</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.0003406565636358403</v>
+        <v>3.194615374249247e-21</v>
       </c>
       <c r="E30" t="n">
-        <v>5.291888876267494</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="31">
@@ -957,13 +957,13 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>0.7085322265458022</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0002602103139767145</v>
+        <v>6.117404547338948e-22</v>
       </c>
       <c r="E31" t="n">
-        <v>5.291207563140222</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="32">
@@ -974,13 +974,13 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0.7084707707480915</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.0001987545162660132</v>
+        <v>1.171428607570567e-22</v>
       </c>
       <c r="E32" t="n">
-        <v>5.291727983768176</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="33">
@@ -991,13 +991,13 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>0.708517708003201</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0001518172611564644</v>
+        <v>2.243181682714838e-23</v>
       </c>
       <c r="E33" t="n">
-        <v>5.291330474735644</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="34">
@@ -1008,13 +1008,13 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>0.7084818529305644</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.0001159621885198306</v>
+        <v>4.295493578650931e-24</v>
       </c>
       <c r="E34" t="n">
-        <v>5.291634109257957</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="35">
@@ -1025,13 +1025,13 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>0.7085092386326286</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D35" t="n">
-        <v>8.857648645569288e-05</v>
+        <v>8.225488477554127e-25</v>
       </c>
       <c r="E35" t="n">
-        <v>5.291402184880917</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="36">
@@ -1042,13 +1042,13 @@
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>0.7084883195463021</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D36" t="n">
-        <v>-6.765740012920079e-05</v>
+        <v>1.575107946398677e-25</v>
       </c>
       <c r="E36" t="n">
-        <v>5.291579337853829</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="37">
@@ -1059,13 +1059,13 @@
         <v>36</v>
       </c>
       <c r="C37" t="n">
-        <v>0.7085042977055429</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D37" t="n">
-        <v>5.167924088839771e-05</v>
+        <v>3.016191742992969e-26</v>
       </c>
       <c r="E37" t="n">
-        <v>5.291444023053571</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="38">
@@ -1076,13 +1076,13 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>0.7084920927174524</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D38" t="n">
-        <v>-3.947425279786777e-05</v>
+        <v>5.775739149370219e-27</v>
       </c>
       <c r="E38" t="n">
-        <v>5.291547381535348</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="39">
@@ -1093,13 +1093,13 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>0.7085014151161101</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D39" t="n">
-        <v>3.015185414012808e-05</v>
+        <v>1.106002720121019e-27</v>
       </c>
       <c r="E39" t="n">
-        <v>5.291468433029752</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="40">
@@ -1110,13 +1110,13 @@
         <v>39</v>
       </c>
       <c r="C40" t="n">
-        <v>0.7084942942390012</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D40" t="n">
-        <v>-2.303097703124299e-05</v>
+        <v>2.117896922419833e-28</v>
       </c>
       <c r="E40" t="n">
-        <v>5.291528736738032</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="41">
@@ -1127,13 +1127,13 @@
         <v>40</v>
       </c>
       <c r="C41" t="n">
-        <v>0.7084997333442737</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D41" t="n">
-        <v>1.759187175878127e-05</v>
+        <v>4.055584396306547e-29</v>
       </c>
       <c r="E41" t="n">
-        <v>5.291482674783969</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="42">
@@ -1144,13 +1144,13 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>0.7084955787321237</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D42" t="n">
-        <v>-1.343725960874021e-05</v>
+        <v>7.766083713258584e-30</v>
       </c>
       <c r="E42" t="n">
-        <v>5.291517858527487</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="43">
@@ -1161,13 +1161,13 @@
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>0.7084987521451314</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D43" t="n">
-        <v>1.026384660105081e-05</v>
+        <v>1.487136016606309e-30</v>
       </c>
       <c r="E43" t="n">
-        <v>5.29149098400827</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="44">
@@ -1178,13 +1178,13 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>0.7084963281709616</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D44" t="n">
-        <v>-7.839872431366297e-06</v>
+        <v>2.847733315199769e-31</v>
       </c>
       <c r="E44" t="n">
-        <v>5.291511511701472</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="45">
@@ -1195,13 +1195,13 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>0.7084981796779053</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D45" t="n">
-        <v>5.988365487715706e-06</v>
+        <v>5.453156230460344e-32</v>
       </c>
       <c r="E45" t="n">
-        <v>5.29149583195661</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="46">
@@ -1212,13 +1212,13 @@
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>0.7084967654292229</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D46" t="n">
-        <v>-4.574116805284849e-06</v>
+        <v>1.044230957831893e-32</v>
       </c>
       <c r="E46" t="n">
-        <v>5.291507808687586</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="47">
@@ -1229,13 +1229,13 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>0.7084978456782099</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D47" t="n">
-        <v>3.493867818204927e-06</v>
+        <v>1.999609487077654e-33</v>
       </c>
       <c r="E47" t="n">
-        <v>5.291498660453975</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="48">
@@ -1246,13 +1246,13 @@
         <v>47</v>
       </c>
       <c r="C48" t="n">
-        <v>0.7084970205456025</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D48" t="n">
-        <v>-2.668735210777387e-06</v>
+        <v>3.829074469418913e-34</v>
       </c>
       <c r="E48" t="n">
-        <v>5.291505648189611</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="49">
@@ -1263,13 +1263,13 @@
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>0.708497650809251</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D49" t="n">
-        <v>2.038471562290415e-06</v>
+        <v>7.332337332417521e-35</v>
       </c>
       <c r="E49" t="n">
-        <v>5.29150031071919</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="50">
@@ -1280,13 +1280,13 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>0.7084971693918133</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D50" t="n">
-        <v>-1.557054124582341e-06</v>
+        <v>1.404077439228352e-35</v>
       </c>
       <c r="E50" t="n">
-        <v>5.291504387662314</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="51">
@@ -1297,13 +1297,13 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>0.7084975371146266</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D51" t="n">
-        <v>1.189331311296862e-06</v>
+        <v>2.688683520647639e-36</v>
       </c>
       <c r="E51" t="n">
-        <v>5.291501273554065</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="52">
@@ -1314,13 +1314,13 @@
         <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>0.7084972562351917</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D52" t="n">
-        <v>-9.084518763411499e-07</v>
+        <v>5.148590008094628e-37</v>
       </c>
       <c r="E52" t="n">
-        <v>5.291503652216687</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="53">
@@ -1331,13 +1331,13 @@
         <v>52</v>
       </c>
       <c r="C53" t="n">
-        <v>0.7084974707804123</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D53" t="n">
-        <v>6.939066557380111e-07</v>
+        <v>9.859092328228613e-38</v>
       </c>
       <c r="E53" t="n">
-        <v>5.291501835312935</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="54">
@@ -1348,13 +1348,13 @@
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>0.7084973069033754</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D54" t="n">
-        <v>-5.300296188886526e-07</v>
+        <v>1.887928566534051e-38</v>
       </c>
       <c r="E54" t="n">
-        <v>5.291503223126246</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="55">
@@ -1365,13 +1365,13 @@
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>0.7084974320782279</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D55" t="n">
-        <v>4.048547663681084e-07</v>
+        <v>3.61521543127258e-39</v>
       </c>
       <c r="E55" t="n">
-        <v>5.291502163067008</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="56">
@@ -1382,13 +1382,13 @@
         <v>55</v>
       </c>
       <c r="C56" t="n">
-        <v>0.7084973364653738</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D56" t="n">
-        <v>-3.092419122559631e-07</v>
+        <v>6.922816279275603e-40</v>
       </c>
       <c r="E56" t="n">
-        <v>5.291502972776541</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="57">
@@ -1399,13 +1399,13 @@
         <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>0.7084974094977309</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D57" t="n">
-        <v>2.362095552036935e-07</v>
+        <v>1.325657796822726e-40</v>
       </c>
       <c r="E57" t="n">
-        <v>5.291502354292716</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="58">
@@ -1416,13 +1416,13 @@
         <v>57</v>
       </c>
       <c r="C58" t="n">
-        <v>0.7084973537131115</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D58" t="n">
-        <v>-1.804249358835508e-07</v>
+        <v>2.53851687432152e-41</v>
       </c>
       <c r="E58" t="n">
-        <v>5.291502826711826</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="59">
@@ -1433,13 +1433,13 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>0.7084973963233081</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D59" t="n">
-        <v>1.37814739344433e-07</v>
+        <v>4.861034225167262e-42</v>
       </c>
       <c r="E59" t="n">
-        <v>5.291502465861955</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="60">
@@ -1450,13 +1450,13 @@
         <v>59</v>
       </c>
       <c r="C60" t="n">
-        <v>0.7084973637761801</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D60" t="n">
-        <v>-1.052676113442643e-07</v>
+        <v>9.308448558004205e-43</v>
       </c>
       <c r="E60" t="n">
-        <v>5.291502741491433</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="61">
@@ -1467,13 +1467,13 @@
         <v>60</v>
       </c>
       <c r="C61" t="n">
-        <v>0.7084973886367885</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D61" t="n">
-        <v>8.040700296812202e-08</v>
+        <v>1.782485177915592e-43</v>
       </c>
       <c r="E61" t="n">
-        <v>5.29150253095621</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="62">
@@ -1484,13 +1484,13 @@
         <v>61</v>
       </c>
       <c r="C62" t="n">
-        <v>0.7084973696474046</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D62" t="n">
-        <v>-6.141761909111371e-08</v>
+        <v>3.413300712455145e-44</v>
       </c>
       <c r="E62" t="n">
-        <v>5.291502691770216</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="63">
@@ -1501,13 +1501,13 @@
         <v>62</v>
       </c>
       <c r="C63" t="n">
-        <v>0.7084973841521451</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D63" t="n">
-        <v>4.691287856576029e-08</v>
+        <v>6.536167536198445e-45</v>
       </c>
       <c r="E63" t="n">
-        <v>5.291502568934978</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="64">
@@ -1518,13 +1518,13 @@
         <v>63</v>
       </c>
       <c r="C64" t="n">
-        <v>0.7084973730729279</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D64" t="n">
-        <v>-3.583366131679749e-08</v>
+        <v>1.251617998536244e-45</v>
       </c>
       <c r="E64" t="n">
-        <v>5.291502662760735</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="65">
@@ -1535,13 +1535,13 @@
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>0.7084973815356129</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D65" t="n">
-        <v>2.737097634661882e-08</v>
+        <v>2.396737240262059e-46</v>
       </c>
       <c r="E65" t="n">
-        <v>5.291502591093412</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="66">
@@ -1552,13 +1552,13 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>0.7084973750715245</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D66" t="n">
-        <v>-2.090688798940128e-08</v>
+        <v>4.58953882540596e-47</v>
       </c>
       <c r="E66" t="n">
-        <v>5.291502645835364</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="67">
@@ -1569,13 +1569,13 @@
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>0.7084973800090163</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D67" t="n">
-        <v>1.596939623559954e-08</v>
+        <v>8.788558994312453e-48</v>
       </c>
       <c r="E67" t="n">
-        <v>5.291502604021589</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="68">
@@ -1586,13 +1586,13 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>0.7084973762375911</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D68" t="n">
-        <v>-1.219797110451684e-08</v>
+        <v>1.68293094654621e-48</v>
       </c>
       <c r="E68" t="n">
-        <v>5.291502635960381</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="69">
@@ -1603,13 +1603,13 @@
         <v>68</v>
       </c>
       <c r="C69" t="n">
-        <v>0.7084973791183347</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D69" t="n">
-        <v>9.31722759685946e-09</v>
+        <v>3.222663206420788e-49</v>
       </c>
       <c r="E69" t="n">
-        <v>5.291502611564439</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="70">
@@ -1620,13 +1620,13 @@
         <v>69</v>
       </c>
       <c r="C70" t="n">
-        <v>0.7084973769179242</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D70" t="n">
-        <v>-7.116817152518144e-09</v>
+        <v>6.17111365343423e-50</v>
       </c>
       <c r="E70" t="n">
-        <v>5.291502630198893</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="71">
@@ -1637,13 +1637,13 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>0.708497378598673</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D71" t="n">
-        <v>5.436068390996945e-09</v>
+        <v>1.181713424093683e-50</v>
       </c>
       <c r="E71" t="n">
-        <v>5.291502615965259</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="72">
@@ -1654,13 +1654,13 @@
         <v>71</v>
       </c>
       <c r="C72" t="n">
-        <v>0.7084973773148596</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D72" t="n">
-        <v>-4.152254989362131e-09</v>
+        <v>2.26287619238076e-51</v>
       </c>
       <c r="E72" t="n">
-        <v>5.291502626837396</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="73">
@@ -1671,13 +1671,13 @@
         <v>72</v>
       </c>
       <c r="C73" t="n">
-        <v>0.7084973782954802</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D73" t="n">
-        <v>3.171634399393595e-09</v>
+        <v>4.333206814478651e-52</v>
       </c>
       <c r="E73" t="n">
-        <v>5.291502618532886</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="74">
@@ -1688,13 +1688,13 @@
         <v>73</v>
       </c>
       <c r="C74" t="n">
-        <v>0.7084973775464487</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D74" t="n">
-        <v>-2.422602847099554e-09</v>
+        <v>8.297705972720218e-53</v>
       </c>
       <c r="E74" t="n">
-        <v>5.291502624876155</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="75">
@@ -1705,13 +1705,13 @@
         <v>74</v>
       </c>
       <c r="C75" t="n">
-        <v>0.7084973781185846</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D75" t="n">
-        <v>1.850466925764023e-09</v>
+        <v>1.588936954951241e-53</v>
       </c>
       <c r="E75" t="n">
-        <v>5.291502620030949</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="76">
@@ -1722,13 +1722,13 @@
         <v>75</v>
       </c>
       <c r="C76" t="n">
-        <v>0.7084973776815676</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D76" t="n">
-        <v>-1.413449937364367e-09</v>
+        <v>3.042673065435277e-54</v>
       </c>
       <c r="E76" t="n">
-        <v>5.291502623731883</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="77">
@@ -1739,13 +1739,13 @@
         <v>76</v>
       </c>
       <c r="C77" t="n">
-        <v>0.7084973780153762</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D77" t="n">
-        <v>1.079641412662091e-09</v>
+        <v>5.826448528544292e-55</v>
       </c>
       <c r="E77" t="n">
-        <v>5.291502620904983</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="78">
@@ -1756,13 +1756,13 @@
         <v>77</v>
       </c>
       <c r="C78" t="n">
-        <v>0.7084973777604018</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D78" t="n">
-        <v>-8.246670426394546e-10</v>
+        <v>1.115713115596253e-55</v>
       </c>
       <c r="E78" t="n">
-        <v>5.291502623064265</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="79">
@@ -1773,13 +1773,13 @@
         <v>78</v>
       </c>
       <c r="C79" t="n">
-        <v>0.7084973779551599</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D79" t="n">
-        <v>6.29908896894295e-10</v>
+        <v>2.136491466825861e-56</v>
       </c>
       <c r="E79" t="n">
-        <v>5.291502621414931</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="80">
@@ -1790,13 +1790,13 @@
         <v>79</v>
       </c>
       <c r="C80" t="n">
-        <v>0.708497377806397</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D80" t="n">
-        <v>-4.811459629608832e-10</v>
+        <v>4.091191296411654e-57</v>
       </c>
       <c r="E80" t="n">
-        <v>5.291502622674749</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="81">
@@ -1807,13 +1807,13 @@
         <v>80</v>
       </c>
       <c r="C81" t="n">
-        <v>0.7084973779200272</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D81" t="n">
-        <v>3.6751574526091e-10</v>
+        <v>7.834267762698588e-58</v>
       </c>
       <c r="E81" t="n">
-        <v>5.291502621712458</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="82">
@@ -1824,13 +1824,13 @@
         <v>81</v>
       </c>
       <c r="C82" t="n">
-        <v>0.7084973778332325</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D82" t="n">
-        <v>-2.807210979736835e-10</v>
+        <v>1.500192656146156e-58</v>
       </c>
       <c r="E82" t="n">
-        <v>5.291502622447489</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="83">
@@ -1841,13 +1841,13 @@
         <v>82</v>
       </c>
       <c r="C83" t="n">
-        <v>0.7084973778995293</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D83" t="n">
-        <v>2.144243773680767e-10</v>
+        <v>2.872735619620468e-59</v>
       </c>
       <c r="E83" t="n">
-        <v>5.291502621886047</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="84">
@@ -1858,13 +1858,13 @@
         <v>83</v>
       </c>
       <c r="C84" t="n">
-        <v>0.7084973778488896</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D84" t="n">
-        <v>-1.637846743270695e-10</v>
+        <v>5.501033421558218e-60</v>
       </c>
       <c r="E84" t="n">
-        <v>5.291502622314896</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="85">
@@ -1875,13 +1875,13 @@
         <v>84</v>
       </c>
       <c r="C85" t="n">
-        <v>0.7084973778875699</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D85" t="n">
-        <v>1.251043368962152e-10</v>
+        <v>1.053399014459203e-60</v>
       </c>
       <c r="E85" t="n">
-        <v>5.291502621987327</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="86">
@@ -1892,13 +1892,13 @@
         <v>85</v>
       </c>
       <c r="C86" t="n">
-        <v>0.7084973778580246</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D86" t="n">
-        <v>-9.55589720117713e-11</v>
+        <v>2.017165500785674e-61</v>
       </c>
       <c r="E86" t="n">
-        <v>5.291502622237536</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="87">
@@ -1909,13 +1909,13 @@
         <v>86</v>
       </c>
       <c r="C87" t="n">
-        <v>0.7084973778805923</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D87" t="n">
-        <v>7.299121164472187e-11</v>
+        <v>3.862692675527943e-62</v>
       </c>
       <c r="E87" t="n">
-        <v>5.291502622046417</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="88">
@@ -1926,13 +1926,13 @@
         <v>87</v>
       </c>
       <c r="C88" t="n">
-        <v>0.7084973778633543</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D88" t="n">
-        <v>-5.575318429185095e-11</v>
+        <v>7.396713209583352e-63</v>
       </c>
       <c r="E88" t="n">
-        <v>5.2915026221924</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="89">
@@ -1943,13 +1943,13 @@
         <v>88</v>
       </c>
       <c r="C89" t="n">
-        <v>0.7084973778765213</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D89" t="n">
-        <v>4.25861893324147e-11</v>
+        <v>1.416404847619596e-63</v>
       </c>
       <c r="E89" t="n">
-        <v>5.291502622080894</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="90">
@@ -1960,13 +1960,13 @@
         <v>89</v>
       </c>
       <c r="C90" t="n">
-        <v>0.7084973778664639</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D90" t="n">
-        <v>-3.252878817382507e-11</v>
+        <v>2.712289412222998e-64</v>
       </c>
       <c r="E90" t="n">
-        <v>5.291502622166067</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="91">
@@ -1977,13 +1977,13 @@
         <v>90</v>
       </c>
       <c r="C91" t="n">
-        <v>0.7084973778741461</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D91" t="n">
-        <v>2.48466011317155e-11</v>
+        <v>5.193793192688026e-65</v>
       </c>
       <c r="E91" t="n">
-        <v>5.291502622101009</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="92">
@@ -1994,13 +1994,13 @@
         <v>91</v>
       </c>
       <c r="C92" t="n">
-        <v>0.7084973778682783</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D92" t="n">
-        <v>-1.897868388141376e-11</v>
+        <v>9.9456524096753e-66</v>
       </c>
       <c r="E92" t="n">
-        <v>5.291502622150703</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="93">
@@ -2011,13 +2011,13 @@
         <v>92</v>
       </c>
       <c r="C93" t="n">
-        <v>0.7084973778727603</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D93" t="n">
-        <v>1.449656795962289e-11</v>
+        <v>1.904504052901779e-66</v>
       </c>
       <c r="E93" t="n">
-        <v>5.291502622112746</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="94">
@@ -2028,13 +2028,13 @@
         <v>93</v>
       </c>
       <c r="C94" t="n">
-        <v>0.7084973778693368</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D94" t="n">
-        <v>-1.107297449710719e-11</v>
+        <v>3.646956014660999e-67</v>
       </c>
       <c r="E94" t="n">
-        <v>5.291502622141738</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="95">
@@ -2045,13 +2045,13 @@
         <v>94</v>
       </c>
       <c r="C95" t="n">
-        <v>0.7084973778719518</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D95" t="n">
-        <v>8.457916698302365e-12</v>
+        <v>6.983596675789262e-68</v>
       </c>
       <c r="E95" t="n">
-        <v>5.291502622119593</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="96">
@@ -2062,13 +2062,13 @@
         <v>95</v>
       </c>
       <c r="C96" t="n">
-        <v>0.7084973778699543</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D96" t="n">
-        <v>-6.460446097300159e-12</v>
+        <v>1.337296702620865e-68</v>
       </c>
       <c r="E96" t="n">
-        <v>5.291502622136509</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="97">
@@ -2079,13 +2079,13 @@
         <v>96</v>
       </c>
       <c r="C97" t="n">
-        <v>0.70849737787148</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D97" t="n">
-        <v>4.934709724031045e-12</v>
+        <v>2.56080434461591e-69</v>
       </c>
       <c r="E97" t="n">
-        <v>5.291502622123588</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="98">
@@ -2096,13 +2096,13 @@
         <v>97</v>
       </c>
       <c r="C98" t="n">
-        <v>0.7084973778703146</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D98" t="n">
-        <v>-3.769300090686748e-12</v>
+        <v>4.903712750171113e-70</v>
       </c>
       <c r="E98" t="n">
-        <v>5.291502622133457</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="99">
@@ -2113,13 +2113,13 @@
         <v>98</v>
       </c>
       <c r="C99" t="n">
-        <v>0.7084973778712048</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D99" t="n">
-        <v>2.879120347134114e-12</v>
+        <v>9.390174140694618e-71</v>
       </c>
       <c r="E99" t="n">
-        <v>5.291502622125918</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
     <row r="100">
@@ -2130,13 +2130,13 @@
         <v>99</v>
       </c>
       <c r="C100" t="n">
-        <v>0.7084973778705249</v>
+        <v>0.5744733400442522</v>
       </c>
       <c r="D100" t="n">
-        <v>-2.199170608294063e-12</v>
+        <v>1.798134900734001e-71</v>
       </c>
       <c r="E100" t="n">
-        <v>5.291502622131676</v>
+        <v>2.425526659955747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>